<commit_message>
Routing to a new Location, tootltip
</commit_message>
<xml_diff>
--- a/Documentation/InitialReview_1.xlsx
+++ b/Documentation/InitialReview_1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>PHASE 1</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t xml:space="preserve">Different Image files can be used to show different icons. But high number of vechicles can be an issue. </t>
-  </si>
-  <si>
-    <t>3``</t>
   </si>
   <si>
     <t xml:space="preserve">Please add labels so that we can related the time slots for a PRV with provided excel
@@ -537,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -563,7 +560,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -582,7 +579,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
@@ -596,29 +593,29 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="75">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45">
@@ -626,13 +623,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -642,12 +639,12 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="28.5">
       <c r="B11" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="75">
@@ -655,13 +652,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30">
@@ -669,13 +666,13 @@
         <v>7</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21">

</xml_diff>